<commit_message>
Updated to version 3.3.2, see CHANGELOG.md for details.
</commit_message>
<xml_diff>
--- a/source/frontend/test_data/test_valid.xlsx
+++ b/source/frontend/test_data/test_valid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bakrnch/Documents/Development/Aws-cloudendure-migration-factory-solution/source/frontend/src/containers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workplace/solutions/Aws-cloudendure-migration-factory-solution/source/frontend/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEFF438-2A26-7747-9A10-C069ECC2046B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD662C-9749-7A4B-8929-53704B348593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21580" yWindow="5540" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8200" yWindow="4040" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_valid" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>server_name</t>
   </si>
   <si>
-    <t>unittest1</t>
-  </si>
-  <si>
     <t>server_os_family</t>
   </si>
   <si>
@@ -49,18 +46,12 @@
     <t>Rehost</t>
   </si>
   <si>
-    <t>Unit testing App 1</t>
-  </si>
-  <si>
     <t>app_name</t>
   </si>
   <si>
     <t>wave_name</t>
   </si>
   <si>
-    <t>Unittest Wave 1</t>
-  </si>
-  <si>
     <t>aws_accountid</t>
   </si>
   <si>
@@ -74,6 +65,15 @@
   </si>
   <si>
     <t>unittest1.testdomain.local</t>
+  </si>
+  <si>
+    <t>unittest1-NEW</t>
+  </si>
+  <si>
+    <t>Unit testing App 1-NEW</t>
+  </si>
+  <si>
+    <t>Unittest Wave 1-NEW</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,8 +926,10 @@
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -935,57 +937,57 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to version 4.0.1, see CHANGELOG.md for details.
</commit_message>
<xml_diff>
--- a/source/frontend/test_data/test_valid.xlsx
+++ b/source/frontend/test_data/test_valid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workplace/solutions/Aws-cloudendure-migration-factory-solution/source/frontend/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bakrnch/Documents/Development/Aws-cloudendure-migration-factory-solution/source/frontend/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD662C-9749-7A4B-8929-53704B348593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8975B03A-94BB-2548-9CE6-7272840BE677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="4040" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>server_name</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Unittest Wave 1-NEW</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>testkey=testvalue;</t>
   </si>
 </sst>
 </file>
@@ -915,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,7 +938,7 @@
     <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,8 +966,11 @@
       <c r="I1" t="s">
         <v>9</v>
       </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -988,6 +997,9 @@
       </c>
       <c r="I2" t="s">
         <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>